<commit_message>
Fix data handling errors when price and sqft are not numbers
</commit_message>
<xml_diff>
--- a/excelFiles/competitor1.xlsx
+++ b/excelFiles/competitor1.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -412,207 +412,432 @@
       <c r="C1" t="str">
         <v>moveInSpecials</v>
       </c>
+      <c r="D1" t="str">
+        <v>Studio</v>
+      </c>
+      <c r="E1" t="str">
+        <v>1 bed</v>
+      </c>
+      <c r="F1" t="str">
+        <v>2 bed</v>
+      </c>
+      <c r="G1" t="str">
+        <v>3 bed</v>
+      </c>
     </row>
     <row r="2" xml:space="preserve">
       <c r="A2" t="str">
-        <v>Maya Apartments</v>
+        <v>Violet on Virgil</v>
       </c>
       <c r="B2" t="str" xml:space="preserve">
-        <v xml:space="preserve">
+        <v xml:space="preserve">Studio: 4
+1 bed: 16
+2 bed: 4
 Percent: %</v>
       </c>
       <c r="C2" t="str">
-        <v>none</v>
+        <v>Up to 4 weeks Free Rent! Contact us to learn more!</v>
+      </c>
+      <c r="D2" t="str" xml:space="preserve">
+        <v xml:space="preserve">5/20: $1825-2092
+($3.97-4.8)</v>
+      </c>
+      <c r="E2" t="str">
+        <v>5/20: $0-2548</v>
+      </c>
+      <c r="F2" t="str" xml:space="preserve">
+        <v xml:space="preserve">5/20: $2699-2799
+($2.81-2.92)</v>
+      </c>
+      <c r="G2" t="str">
+        <v>n/a</v>
       </c>
     </row>
     <row r="3" xml:space="preserve">
       <c r="A3" t="str">
-        <v>New Hampshire Terrace</v>
+        <v>Plaza at Lafayette</v>
       </c>
       <c r="B3" t="str" xml:space="preserve">
-        <v xml:space="preserve">Studio: 1
-2 bed: 1
+        <v xml:space="preserve">1 bed: 1
+2 bed: 4
 Percent: %</v>
       </c>
       <c r="C3" t="str">
-        <v>none</v>
+        <v>Up to 1 Month Free! *Restrictions Apply, Contact for Details</v>
+      </c>
+      <c r="D3" t="str">
+        <v>n/a</v>
+      </c>
+      <c r="E3" t="str" xml:space="preserve">
+        <v xml:space="preserve">5/20: $2200
+($2.91)</v>
+      </c>
+      <c r="F3" t="str" xml:space="preserve">
+        <v xml:space="preserve">5/20: $2771-2991
+($3.03-3.19)</v>
+      </c>
+      <c r="G3" t="str">
+        <v>n/a</v>
       </c>
     </row>
     <row r="4" xml:space="preserve">
       <c r="A4" t="str">
-        <v>Violet on Virgil</v>
+        <v>The Pearl</v>
       </c>
       <c r="B4" t="str" xml:space="preserve">
-        <v xml:space="preserve">Studio: 4
-1 bed: 17
-2 bed: 4
+        <v xml:space="preserve">Studio: 7
+1 bed: 7
+2 bed: 3
 Percent: %</v>
       </c>
       <c r="C4" t="str">
-        <v>Up to 4 weeks Free Rent! Contact us to learn more!</v>
+        <v>$500 Look &amp; Lease Special* Restrictions Apply</v>
+      </c>
+      <c r="D4" t="str" xml:space="preserve">
+        <v xml:space="preserve">5/20: $2335-2540
+($5.37-5.99)</v>
+      </c>
+      <c r="E4" t="str" xml:space="preserve">
+        <v xml:space="preserve">5/20: $2991-3179
+($5.03-5.53)</v>
+      </c>
+      <c r="F4" t="str" xml:space="preserve">
+        <v xml:space="preserve">5/20: $3517-4307
+($4.04-4.21)</v>
+      </c>
+      <c r="G4" t="str">
+        <v>n/a</v>
       </c>
     </row>
     <row r="5" xml:space="preserve">
       <c r="A5" t="str">
-        <v>Plaza at Lafayette</v>
+        <v>Mariposa on 3rd</v>
       </c>
       <c r="B5" t="str" xml:space="preserve">
-        <v xml:space="preserve">1 bed: 2
+        <v xml:space="preserve">1 bed: 11
 2 bed: 3
 Percent: %</v>
       </c>
       <c r="C5" t="str">
-        <v>Up to 1 Month Free! *Restrictions Apply, Contact for Details</v>
+        <v>none</v>
+      </c>
+      <c r="D5" t="str">
+        <v>n/a</v>
+      </c>
+      <c r="E5" t="str">
+        <v>5/20: $0-2945</v>
+      </c>
+      <c r="F5" t="str" xml:space="preserve">
+        <v xml:space="preserve">5/20: $3249-3380
+($3.38-3.69)</v>
+      </c>
+      <c r="G5" t="str">
+        <v>n/a</v>
       </c>
     </row>
     <row r="6" xml:space="preserve">
       <c r="A6" t="str">
-        <v>Next on Sixth</v>
+        <v>Kingsley Plaza</v>
       </c>
       <c r="B6" t="str" xml:space="preserve">
-        <v xml:space="preserve">Studio: 12
-1 bed: 4
-2 bed: 3
+        <v xml:space="preserve">Studio: 5
+1 bed: 6
 Percent: %</v>
       </c>
       <c r="C6" t="str">
-        <v>none</v>
+        <v>Look &amp; Lease on the Same Day for $1,000 Off Select Apartments!</v>
+      </c>
+      <c r="D6" t="str" xml:space="preserve">
+        <v xml:space="preserve">5/20: $1900
+($4.22)</v>
+      </c>
+      <c r="E6" t="str" xml:space="preserve">
+        <v xml:space="preserve">5/20: $2000-2500
+($2.67-3.13)</v>
+      </c>
+      <c r="F6" t="str">
+        <v>n/a</v>
+      </c>
+      <c r="G6" t="str">
+        <v>n/a</v>
       </c>
     </row>
     <row r="7" xml:space="preserve">
       <c r="A7" t="str">
-        <v>3033 Wilshire</v>
+        <v>Wilshire Valencia</v>
       </c>
       <c r="B7" t="str" xml:space="preserve">
-        <v xml:space="preserve">Studio: 4
+        <v xml:space="preserve">Studio: 5
+1 bed: 8
+2 bed: 5
+Percent: %</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Up to $1,500 Look and Lease Special! *Restrictions Apply, Contact for Details</v>
+      </c>
+      <c r="D7" t="str" xml:space="preserve">
+        <v xml:space="preserve">5/20: $1999-2193
+($3.22-3.5)</v>
+      </c>
+      <c r="E7" t="str" xml:space="preserve">
+        <v xml:space="preserve">5/20: $2427-2708
+($3.17-3.89)</v>
+      </c>
+      <c r="F7" t="str" xml:space="preserve">
+        <v xml:space="preserve">5/20: $3032-3441
+($2.89-3.69)</v>
+      </c>
+      <c r="G7" t="str">
+        <v>n/a</v>
+      </c>
+    </row>
+    <row r="8" xml:space="preserve">
+      <c r="A8" t="str">
+        <v>Wilshire Vermont</v>
+      </c>
+      <c r="B8" t="str" xml:space="preserve">
+        <v xml:space="preserve">Studio: 8
 1 bed: 9
 2 bed: 7
 Percent: %</v>
       </c>
-      <c r="C7" t="str">
-        <v>Save up to 8 Weeks off rent! Minimum 12 month lease term required.</v>
-      </c>
-    </row>
-    <row r="8" xml:space="preserve">
-      <c r="A8" t="str">
-        <v>Kingsley Tower Apartments</v>
-      </c>
-      <c r="B8" t="str" xml:space="preserve">
-        <v xml:space="preserve">Studio: 1
-2 bed: 1
-Percent: %</v>
-      </c>
       <c r="C8" t="str">
-        <v>none</v>
+        <v>1 Month Free + $500 Look and Lease on Select Units! AND Furnished Studio and 1-Bedroom Units Available! *Restrictions apply. Please call for details.</v>
+      </c>
+      <c r="D8" t="str" xml:space="preserve">
+        <v xml:space="preserve">5/20: $1797-1905
+($3.57-3.83)</v>
+      </c>
+      <c r="E8" t="str" xml:space="preserve">
+        <v xml:space="preserve">5/20: $2493-2781
+($2.86-3.65)</v>
+      </c>
+      <c r="F8" t="str">
+        <v>5/20: $0-3330</v>
+      </c>
+      <c r="G8" t="str">
+        <v>n/a</v>
       </c>
     </row>
     <row r="9" xml:space="preserve">
       <c r="A9" t="str">
-        <v>The Vermont</v>
+        <v>Kodo</v>
       </c>
       <c r="B9" t="str" xml:space="preserve">
-        <v xml:space="preserve">Studio: 7
-1 bed: 14
-2 bed: 13
-Percent: %</v>
-      </c>
-      <c r="C9" t="str">
-        <v>none</v>
-      </c>
-    </row>
-    <row r="10" xml:space="preserve">
-      <c r="A10" t="str">
-        <v>Radius Koreatown</v>
-      </c>
-      <c r="B10" t="str" xml:space="preserve">
-        <v xml:space="preserve">Studio: 1
-1 bed: 9
-Percent: %</v>
-      </c>
-      <c r="C10" t="str">
-        <v>Up to 1 month off select apartment homes. Offer valid on new leases only. Transfers excluded. [Offer good thru Jun 01, 2024]</v>
-      </c>
-    </row>
-    <row r="11" xml:space="preserve">
-      <c r="A11" t="str">
-        <v>Mariposa on 3rd</v>
-      </c>
-      <c r="B11" t="str" xml:space="preserve">
-        <v xml:space="preserve">1 bed: 11
-2 bed: 3
-Percent: %</v>
-      </c>
-      <c r="C11" t="str">
-        <v>none</v>
-      </c>
-    </row>
-    <row r="12" xml:space="preserve">
-      <c r="A12" t="str">
-        <v>Kingsley Plaza</v>
-      </c>
-      <c r="B12" t="str" xml:space="preserve">
-        <v xml:space="preserve">Studio: 5
-1 bed: 6
-Percent: %</v>
-      </c>
-      <c r="C12" t="str">
-        <v>Look &amp; Lease on the Same Day for $1,000 Off Select Apartments!</v>
-      </c>
-    </row>
-    <row r="13" xml:space="preserve">
-      <c r="A13" t="str">
-        <v>Kodo</v>
-      </c>
-      <c r="B13" t="str" xml:space="preserve">
         <v xml:space="preserve">Studio: 2
 1 bed: 3
 2 bed: 4
 Percent: %</v>
       </c>
+      <c r="C9" t="str">
+        <v>RECEIVE ONE MONTH RENT FOR IMMEDIATE MOVE INS, CONTACT US TO FIND OUT HOW!</v>
+      </c>
+      <c r="D9" t="str" xml:space="preserve">
+        <v xml:space="preserve">5/20: $2099-2199
+($3.62-3.94)</v>
+      </c>
+      <c r="E9" t="str" xml:space="preserve">
+        <v xml:space="preserve">5/20: $2499
+($3.96-3.98)</v>
+      </c>
+      <c r="F9" t="str" xml:space="preserve">
+        <v xml:space="preserve">5/20: $3150-3499
+($3.34-3.62)</v>
+      </c>
+      <c r="G9" t="str">
+        <v>n/a</v>
+      </c>
+    </row>
+    <row r="10" xml:space="preserve">
+      <c r="A10" t="str">
+        <v>3033 Wilshire</v>
+      </c>
+      <c r="B10" t="str" xml:space="preserve">
+        <v xml:space="preserve">Studio: 4
+1 bed: 10
+2 bed: 8
+Percent: %</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Save up to 8 Weeks off rent! Minimum 12 month lease term required.</v>
+      </c>
+      <c r="D10" t="str" xml:space="preserve">
+        <v xml:space="preserve">5/20: $2296-2726
+($3.73-4.43)</v>
+      </c>
+      <c r="E10" t="str" xml:space="preserve">
+        <v xml:space="preserve">5/20: $2781-3381
+($3.13-4.07)</v>
+      </c>
+      <c r="F10" t="str" xml:space="preserve">
+        <v xml:space="preserve">5/20: $3709-6831
+($2.97-3.74)</v>
+      </c>
+      <c r="G10" t="str">
+        <v>n/a</v>
+      </c>
+    </row>
+    <row r="11" xml:space="preserve">
+      <c r="A11" t="str">
+        <v>New Hampshire Terrace</v>
+      </c>
+      <c r="B11" t="str" xml:space="preserve">
+        <v xml:space="preserve">Studio: 1
+2 bed: 1
+Percent: %</v>
+      </c>
+      <c r="C11" t="str">
+        <v>none</v>
+      </c>
+      <c r="D11" t="str" xml:space="preserve">
+        <v xml:space="preserve">5/20: $1600
+($3.33)</v>
+      </c>
+      <c r="E11" t="str">
+        <v>n/a</v>
+      </c>
+      <c r="F11" t="str" xml:space="preserve">
+        <v xml:space="preserve">5/20: $2655
+($Infinity)</v>
+      </c>
+      <c r="G11" t="str">
+        <v>n/a</v>
+      </c>
+    </row>
+    <row r="12" xml:space="preserve">
+      <c r="A12" t="str">
+        <v>Next on Sixth</v>
+      </c>
+      <c r="B12" t="str" xml:space="preserve">
+        <v xml:space="preserve">Studio: 11
+1 bed: 3
+2 bed: 3
+Percent: %</v>
+      </c>
+      <c r="C12" t="str">
+        <v>none</v>
+      </c>
+      <c r="D12" t="str" xml:space="preserve">
+        <v xml:space="preserve">5/20: $2005-2150
+($3.69-4.63)</v>
+      </c>
+      <c r="E12" t="str" xml:space="preserve">
+        <v xml:space="preserve">5/20: $2650-3257
+($2.98-3.98)</v>
+      </c>
+      <c r="F12" t="str" xml:space="preserve">
+        <v xml:space="preserve">5/20: $3095-3432
+($3.19-3.36)</v>
+      </c>
+      <c r="G12" t="str">
+        <v>n/a</v>
+      </c>
+    </row>
+    <row r="13" xml:space="preserve">
+      <c r="A13" t="str">
+        <v>Kingsley Tower Apartments</v>
+      </c>
+      <c r="B13" t="str" xml:space="preserve">
+        <v xml:space="preserve">Studio: 1
+2 bed: 1
+Percent: %</v>
+      </c>
       <c r="C13" t="str">
-        <v>RECEIVE ONE MONTH RENT FOR IMMEDIATE MOVE INS, CONTACT US TO FIND OUT HOW!</v>
+        <v>none</v>
+      </c>
+      <c r="D13" t="str" xml:space="preserve">
+        <v xml:space="preserve">5/20: $2270
+($4.05)</v>
+      </c>
+      <c r="E13" t="str">
+        <v>n/a</v>
+      </c>
+      <c r="F13" t="str" xml:space="preserve">
+        <v xml:space="preserve">5/20: $3145
+($2.86)</v>
+      </c>
+      <c r="G13" t="str">
+        <v>n/a</v>
       </c>
     </row>
     <row r="14" xml:space="preserve">
       <c r="A14" t="str">
-        <v>Wilshire Valencia</v>
+        <v>Radius Koreatown</v>
       </c>
       <c r="B14" t="str" xml:space="preserve">
-        <v xml:space="preserve">Studio: 5
+        <v xml:space="preserve">Studio: 1
 1 bed: 9
-2 bed: 5
 Percent: %</v>
       </c>
       <c r="C14" t="str">
-        <v>Up to $1,500 Look and Lease Special! *Restrictions Apply, Contact for Details</v>
+        <v>Up to 1 month off select apartment homes. Offer valid on new leases only. Transfers excluded. [Offer good thru Jun 01, 2024]</v>
+      </c>
+      <c r="D14" t="str" xml:space="preserve">
+        <v xml:space="preserve">5/20: $2135
+($3.69)</v>
+      </c>
+      <c r="E14" t="str" xml:space="preserve">
+        <v xml:space="preserve">5/20: $2058-2356
+($3.15-3.8)</v>
+      </c>
+      <c r="F14" t="str">
+        <v>n/a</v>
+      </c>
+      <c r="G14" t="str">
+        <v>n/a</v>
       </c>
     </row>
     <row r="15" xml:space="preserve">
       <c r="A15" t="str">
-        <v>The Pearl</v>
+        <v>Maya Apartments</v>
       </c>
       <c r="B15" t="str" xml:space="preserve">
-        <v xml:space="preserve">Studio: 7
-1 bed: 7
-2 bed: 3
+        <v xml:space="preserve">
 Percent: %</v>
       </c>
       <c r="C15" t="str">
-        <v>$500 Look &amp; Lease Special* Restrictions Apply</v>
+        <v>none</v>
+      </c>
+      <c r="D15" t="str">
+        <v>n/a</v>
+      </c>
+      <c r="E15" t="str">
+        <v>n/a</v>
+      </c>
+      <c r="F15" t="str">
+        <v>n/a</v>
+      </c>
+      <c r="G15" t="str">
+        <v>n/a</v>
       </c>
     </row>
     <row r="16" xml:space="preserve">
       <c r="A16" t="str">
-        <v>Wilshire Vermont</v>
+        <v>The Vermont</v>
       </c>
       <c r="B16" t="str" xml:space="preserve">
         <v xml:space="preserve">Studio: 8
-1 bed: 9
-2 bed: 7
+1 bed: 14
+2 bed: 13
 Percent: %</v>
       </c>
       <c r="C16" t="str">
-        <v>1 Month Free + $500 Look and Lease on Select Units! AND Furnished Studio and 1-Bedroom Units Available! *Restrictions apply. Please call for details.</v>
+        <v>none</v>
+      </c>
+      <c r="D16" t="str" xml:space="preserve">
+        <v xml:space="preserve">5/20: $2440-2870
+($3.18-3.74)</v>
+      </c>
+      <c r="E16" t="str" xml:space="preserve">
+        <v xml:space="preserve">5/20: $2425-3295
+($3.85-5.08)</v>
+      </c>
+      <c r="F16" t="str" xml:space="preserve">
+        <v xml:space="preserve">5/20: $3500-4434
+($3.63-4.4)</v>
+      </c>
+      <c r="G16" t="str">
+        <v>n/a</v>
       </c>
     </row>
     <row r="17" xml:space="preserve">
@@ -628,10 +853,25 @@
       <c r="C17" t="str">
         <v>New Special New Specials - $99 Deposit On Approved Credit + 1 Month Free Credit + 3 Months Free Parking. For A Limited Time Only. Pricing and Specials Are Subject To Change.</v>
       </c>
+      <c r="D17" t="str" xml:space="preserve">
+        <v xml:space="preserve">5/20: $2288
+($4.57)</v>
+      </c>
+      <c r="E17" t="str" xml:space="preserve">
+        <v xml:space="preserve">5/20: $2548-2675
+($3.37-3.82)</v>
+      </c>
+      <c r="F17" t="str" xml:space="preserve">
+        <v xml:space="preserve">5/20: $2898-3106
+($2.91-3.11)</v>
+      </c>
+      <c r="G17" t="str">
+        <v>n/a</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C17"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G17"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implement calculating vacancy percentage by passing in the total unit counts for each building
</commit_message>
<xml_diff>
--- a/excelFiles/competitor1.xlsx
+++ b/excelFiles/competitor1.xlsx
@@ -430,25 +430,25 @@
         <v>The Pearl</v>
       </c>
       <c r="B2" t="str" xml:space="preserve">
-        <v xml:space="preserve">Studio: 6
+        <v xml:space="preserve">Studio: 7
 1 bed: 4
 2 bed: 3
-Percent: %</v>
+Percent: 4.0%</v>
       </c>
       <c r="C2" t="str">
         <v>4 Weeks Free Plus $750 Look and Lease* Restrictions Apply</v>
       </c>
       <c r="D2" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $2341-2546
-($5.38-6.01)</v>
+        <v xml:space="preserve">6/16: $2217-2424
+($5.1-5.97)</v>
       </c>
       <c r="E2" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $2759-2939
-($4.8-5.11)</v>
+        <v xml:space="preserve">6/16: $2861-3034
+($4.98-5.21)</v>
       </c>
       <c r="F2" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $3694-4484
-($4.21-4.43)</v>
+        <v xml:space="preserve">6/16: $3510-4300
+($4.03-4.21)</v>
       </c>
       <c r="G2" t="str">
         <v>n/a</v>
@@ -459,25 +459,25 @@
         <v>3033 Wilshire</v>
       </c>
       <c r="B3" t="str" xml:space="preserve">
-        <v xml:space="preserve">Studio: 5
-1 bed: 13
-2 bed: 7
-Percent: %</v>
+        <v xml:space="preserve">Studio: 4
+1 bed: 11
+2 bed: 8
+Percent: 12.1%</v>
       </c>
       <c r="C3" t="str">
-        <v>none</v>
+        <v>Save 8 weeks off rent! Minimum 13 month lease term required.</v>
       </c>
       <c r="D3" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $2193-2713
-($3.57-4.35)</v>
+        <v xml:space="preserve">6/16: $2208-2688
+($3.59-4.37)</v>
       </c>
       <c r="E3" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $2739-3308
-($2.97-3.94)</v>
+        <v xml:space="preserve">6/16: $2566-3496
+($2.91-4.16)</v>
       </c>
       <c r="F3" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $3498-6596
-($2.71-3.62)</v>
+        <v xml:space="preserve">6/16: $3693-7411
+($2.68-4.07)</v>
       </c>
       <c r="G3" t="str">
         <v>n/a</v>
@@ -488,25 +488,25 @@
         <v>Next on Sixth</v>
       </c>
       <c r="B4" t="str" xml:space="preserve">
-        <v xml:space="preserve">Studio: 9
-1 bed: 10
-2 bed: 2
-Percent: %</v>
+        <v xml:space="preserve">Studio: 6
+1 bed: 18
+2 bed: 3
+Percent: 6.8%</v>
       </c>
       <c r="C4" t="str">
         <v>none</v>
       </c>
       <c r="D4" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $1995-2165
-($3.73-4.71)</v>
+        <v xml:space="preserve">6/16: $2050-2225
+($3.84-4.85)</v>
       </c>
       <c r="E4" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $2675-3462
-($3.05-4.53)</v>
+        <v xml:space="preserve">6/16: $2570-3442
+($3.04-4.36)</v>
       </c>
       <c r="F4" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $3140-3452
-($3.21-3.37)</v>
+        <v xml:space="preserve">6/16: $3105-3407
+($3.16-3.51)</v>
       </c>
       <c r="G4" t="str">
         <v>n/a</v>
@@ -517,25 +517,25 @@
         <v>Avana on Wilshire</v>
       </c>
       <c r="B5" t="str" xml:space="preserve">
-        <v xml:space="preserve">Studio: 1
+        <v xml:space="preserve">Studio: 2
 1 bed: 4
-2 bed: 7
-Percent: %</v>
+2 bed: 6
+Percent: 7.5%</v>
       </c>
       <c r="C5" t="str">
         <v>New Special New Specials - $99 Deposit On Approved Credit + 1 Month Free Credit + 3 Months Free Parking. For A Limited Time Only. Pricing and Specials Are Subject To Change.</v>
       </c>
       <c r="D5" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $2201
-($4.39)</v>
+        <v xml:space="preserve">6/16: $2312-2406
+($4.61-4.75)</v>
       </c>
       <c r="E5" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $2610-2736
-($3.45-3.91)</v>
+        <v xml:space="preserve">6/16: $2572-2643
+($3.4-3.86)</v>
       </c>
       <c r="F5" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $3206-3264
-($3.18-3.27)</v>
+        <v xml:space="preserve">6/16: $3441-3508
+($3.41-3.51)</v>
       </c>
       <c r="G5" t="str">
         <v>n/a</v>
@@ -546,23 +546,25 @@
         <v>Radius Koreatown</v>
       </c>
       <c r="B6" t="str" xml:space="preserve">
-        <v xml:space="preserve">Studio: 4
-1 bed: 5
-Percent: %</v>
+        <v xml:space="preserve">Studio: 6
+1 bed: 6
+2 bed: 1
+Percent: 4.3%</v>
       </c>
       <c r="C6" t="str">
-        <v>Up to 1 month off select apartment homes. Offer valid on new leases only. Transfers excluded. [Offer good thru Jun 15, 2024]</v>
+        <v>Up to 1 month off select apartment homes. Offer valid on new leases only. Transfers excluded. [Offer good thru Jun 29, 2024]</v>
       </c>
       <c r="D6" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $2025-2170
-($3.75-5.07)</v>
+        <v xml:space="preserve">6/16: $1826-2060
+($3.55-4.77)</v>
       </c>
       <c r="E6" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $2197-2431
-($3.64-3.92)</v>
-      </c>
-      <c r="F6" t="str">
-        <v>n/a</v>
+        <v xml:space="preserve">6/16: $2219-2382
+($3.82-4.09)</v>
+      </c>
+      <c r="F6" t="str" xml:space="preserve">
+        <v xml:space="preserve">6/16: $3386
+($3.51)</v>
       </c>
       <c r="G6" t="str">
         <v>n/a</v>
@@ -573,25 +575,25 @@
         <v>Wilshire Vermont</v>
       </c>
       <c r="B7" t="str" xml:space="preserve">
-        <v xml:space="preserve">Studio: 6
-1 bed: 8
-2 bed: 7
-Percent: %</v>
+        <v xml:space="preserve">Studio: 7
+1 bed: 7
+2 bed: 6
+Percent: 4.5%</v>
       </c>
       <c r="C7" t="str">
         <v>One month free plus $1000 Look &amp; Lease on select units! *Restrictions apply. Please call for details.*</v>
       </c>
       <c r="D7" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $1995-2090
-($3.97-4.21)</v>
+        <v xml:space="preserve">6/16: $1856-2045
+($3.69-4.12)</v>
       </c>
       <c r="E7" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $2369-2708
-($2.84-3.34)</v>
+        <v xml:space="preserve">6/16: $2355-2702
+($2.97-3.3)</v>
       </c>
       <c r="F7" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $3266-3371
-($3.08-3.22)</v>
+        <v xml:space="preserve">6/16: $3119-3275
+($2.94-3.08)</v>
       </c>
       <c r="G7" t="str">
         <v>n/a</v>
@@ -603,24 +605,24 @@
       </c>
       <c r="B8" t="str" xml:space="preserve">
         <v xml:space="preserve">Studio: 7
-1 bed: 16
-2 bed: 11
-Percent: %</v>
+1 bed: 15
+2 bed: 14
+Percent: 7.8%</v>
       </c>
       <c r="C8" t="str">
-        <v>1 month FREE + add'l look &amp; lease incentives! *Offer subject to change. Some restrictions may apply. Contact office for details.</v>
+        <v>6 weeks FREE on all apts! Look &amp; lease &amp; receive 2 weeks free *Offers subject to change. Some restrictions may apply. Contact office for details</v>
       </c>
       <c r="D8" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $2535-2900
-($3.3-3.78)</v>
+        <v xml:space="preserve">6/16: $2695-2915
+($3.51-3.8)</v>
       </c>
       <c r="E8" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $2405-3275
-($3.89-5.05)</v>
+        <v xml:space="preserve">6/16: $2470-3340
+($4.01-5.15)</v>
       </c>
       <c r="F8" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $3705-4554
-($3.76-4.52)</v>
+        <v xml:space="preserve">6/16: $3470-4314
+($3.52-4.28)</v>
       </c>
       <c r="G8" t="str">
         <v>n/a</v>
@@ -631,25 +633,23 @@
         <v>Violet on Virgil</v>
       </c>
       <c r="B9" t="str" xml:space="preserve">
-        <v xml:space="preserve">Studio: 8
-1 bed: 11
-2 bed: 2
-Percent: %</v>
+        <v xml:space="preserve">Studio: 6
+1 bed: 7
+Percent: 4.3%</v>
       </c>
       <c r="C9" t="str">
         <v>Up to 4 weeks Free Rent! Contact us to learn more!</v>
       </c>
       <c r="D9" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $1825-2170
-($3.97-4.86)</v>
+        <v xml:space="preserve">6/16: $1599-1950
+($3.48-4.24)</v>
       </c>
       <c r="E9" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $2079-2548
-($3.1-3.8)</v>
-      </c>
-      <c r="F9" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $2700-2799
-($2.81-2.92)</v>
+        <v xml:space="preserve">6/16: $1825-1999
+($2.72-2.98)</v>
+      </c>
+      <c r="F9" t="str">
+        <v>n/a</v>
       </c>
       <c r="G9" t="str">
         <v>n/a</v>
@@ -660,25 +660,25 @@
         <v>Wilshire Valencia</v>
       </c>
       <c r="B10" t="str" xml:space="preserve">
-        <v xml:space="preserve">Studio: 6
-1 bed: 8
-2 bed: 3
-Percent: %</v>
+        <v xml:space="preserve">Studio: 5
+1 bed: 9
+2 bed: 4
+Percent: 8.2%</v>
       </c>
       <c r="C10" t="str">
         <v>6 Weeks Free on All Vacant Units. *Restrictions Apply, Contact Leasing Office for Details</v>
       </c>
       <c r="D10" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $2017-2193
-($3.25-3.5)</v>
+        <v xml:space="preserve">6/16: $1916-2193
+($3.09-3.5)</v>
       </c>
       <c r="E10" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $2611-2731
-($3.47-3.89)</v>
+        <v xml:space="preserve">6/16: $2372-2708
+($3.17-3.89)</v>
       </c>
       <c r="F10" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $2749-3441
-($2.9-3.69)</v>
+        <v xml:space="preserve">6/16: $2808-3441
+($2.78-3.18)</v>
       </c>
       <c r="G10" t="str">
         <v>n/a</v>
@@ -689,25 +689,25 @@
         <v>Kodo</v>
       </c>
       <c r="B11" t="str" xml:space="preserve">
-        <v xml:space="preserve">Studio: 1
-1 bed: 2
-2 bed: 4
-Percent: %</v>
+        <v xml:space="preserve">Studio: 3
+1 bed: 1
+2 bed: 3
+Percent: 11.7%</v>
       </c>
       <c r="C11" t="str">
         <v>none</v>
       </c>
       <c r="D11" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $2099
-($3.94)</v>
+        <v xml:space="preserve">6/16: $1925-2149
+($3.61-4.61)</v>
       </c>
       <c r="E11" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $2399
-($3.81-3.82)</v>
+        <v xml:space="preserve">6/16: $2199
+($3.5)</v>
       </c>
       <c r="F11" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $2899-3399
-($3.18-3.52)</v>
+        <v xml:space="preserve">6/16: $3021-3200
+($3.2-3.66)</v>
       </c>
       <c r="G11" t="str">
         <v>n/a</v>
@@ -719,8 +719,8 @@
       </c>
       <c r="B12" t="str" xml:space="preserve">
         <v xml:space="preserve">1 bed: 1
-2 bed: 4
-Percent: %</v>
+2 bed: 5
+Percent: 10.7%</v>
       </c>
       <c r="C12" t="str">
         <v>6 Weeks Free for New Move In's! *Restrictions Apply, Contact for Details</v>
@@ -729,11 +729,11 @@
         <v>n/a</v>
       </c>
       <c r="E12" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $2200
-($2.91)</v>
+        <v xml:space="preserve">6/16: $2210
+($2.93)</v>
       </c>
       <c r="F12" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $2654-2991
+        <v xml:space="preserve">6/16: $2599-2991
 ($2.93-3.19)</v>
       </c>
       <c r="G12" t="str">
@@ -747,18 +747,18 @@
       <c r="B13" t="str" xml:space="preserve">
         <v xml:space="preserve">Studio: 5
 1 bed: 6
-Percent: %</v>
+Percent: 6.8%</v>
       </c>
       <c r="C13" t="str">
         <v>Look &amp; Lease on the Same Day for $1,000 Off Select Apartments!</v>
       </c>
       <c r="D13" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $1900
+        <v xml:space="preserve">6/16: $1900
 ($4.22)</v>
       </c>
       <c r="E13" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $2000-2500
-($2.67-3.13)</v>
+        <v xml:space="preserve">6/16: $2200-2500
+($2.93-3.13)</v>
       </c>
       <c r="F13" t="str">
         <v>n/a</v>
@@ -773,21 +773,23 @@
       </c>
       <c r="B14" t="str" xml:space="preserve">
         <v xml:space="preserve">Studio: 3
+1 bed: 1
 2 bed: 1
-Percent: %</v>
+Percent: 4.9%</v>
       </c>
       <c r="C14" t="str">
         <v>none</v>
       </c>
       <c r="D14" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $2235
-($3.73-3.99)</v>
-      </c>
-      <c r="E14" t="str">
-        <v>n/a</v>
+        <v xml:space="preserve">6/16: $2245-2295
+($3.74-4.01)</v>
+      </c>
+      <c r="E14" t="str" xml:space="preserve">
+        <v xml:space="preserve">6/16: $2595
+($3.33)</v>
       </c>
       <c r="F14" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $3090
+        <v xml:space="preserve">6/16: $3090
 ($2.81)</v>
       </c>
       <c r="G14" t="str">
@@ -800,21 +802,23 @@
       </c>
       <c r="B15" t="str" xml:space="preserve">
         <v xml:space="preserve">Studio: 1
+1 bed: 1
 2 bed: 1
-Percent: %</v>
+Percent: 3.2%</v>
       </c>
       <c r="C15" t="str">
         <v>none</v>
       </c>
       <c r="D15" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $1600
+        <v xml:space="preserve">6/16: $1600
 ($3.33)</v>
       </c>
-      <c r="E15" t="str">
-        <v>n/a</v>
+      <c r="E15" t="str" xml:space="preserve">
+        <v xml:space="preserve">6/16: $1900
+($3.13)</v>
       </c>
       <c r="F15" t="str">
-        <v>6/2: $2655</v>
+        <v>6/16: $2655</v>
       </c>
       <c r="G15" t="str">
         <v>n/a</v>
@@ -825,9 +829,9 @@
         <v>Mariposa on 3rd</v>
       </c>
       <c r="B16" t="str" xml:space="preserve">
-        <v xml:space="preserve">1 bed: 8
-2 bed: 2
-Percent: %</v>
+        <v xml:space="preserve">1 bed: 5
+2 bed: 3
+Percent: 6.6%</v>
       </c>
       <c r="C16" t="str">
         <v>none</v>
@@ -836,12 +840,12 @@
         <v>n/a</v>
       </c>
       <c r="E16" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $2489-2805
-($3.36-3.75)</v>
+        <v xml:space="preserve">6/16: $2524-2831
+($3.41-3.87)</v>
       </c>
       <c r="F16" t="str" xml:space="preserve">
-        <v xml:space="preserve">6/2: $3290-3310
-($3.68-3.74)</v>
+        <v xml:space="preserve">6/16: $3370-3563
+($3.56-3.83)</v>
       </c>
       <c r="G16" t="str">
         <v>n/a</v>

</xml_diff>